<commit_message>
updated pronoun list xl sheet
</commit_message>
<xml_diff>
--- a/ListOfPronouns.xlsx
+++ b/ListOfPronouns.xlsx
@@ -890,7 +890,6 @@
       <c r="A13" s="3"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A1:A1048576">
     <sortCondition ref="A1:A1048576"/>
   </sortState>
@@ -910,7 +909,7 @@
   <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="E1" sqref="E1:E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2076,7 +2075,6 @@
     <row r="79" spans="1:5" ht="16"/>
     <row r="80" spans="1:5" ht="16"/>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>